<commit_message>
9/22/2013 fixed usb connection 1-VCC 2-data- 3-data+ 5-GND added resistor network for ipod iphone charging Signed-off-by: goose1987 <phamh1987@gmail.com>
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BOM" localSheetId="0">Sheet1!$A$1:$M$31</definedName>
+    <definedName name="BOM" localSheetId="0">Sheet1!$A$1:$I$31</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="89">
   <si>
     <t>Part</t>
   </si>
@@ -74,21 +74,9 @@
     <t>MPN</t>
   </si>
   <si>
-    <t>OC_FARNELL</t>
-  </si>
-  <si>
     <t>OC_NEWARK</t>
   </si>
   <si>
-    <t>SPICEMODEL</t>
-  </si>
-  <si>
-    <t>SPICEPREFIX</t>
-  </si>
-  <si>
-    <t>SPICETYPE</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -158,9 +146,6 @@
     <t>SSOP28</t>
   </si>
   <si>
-    <t>Source: http://www.ftdichip.com/Documents/DataSheets/DS_FT232R_v104.pdf</t>
-  </si>
-  <si>
     <t>91K9918</t>
   </si>
   <si>
@@ -176,15 +161,6 @@
     <t>LED</t>
   </si>
   <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>diode</t>
-  </si>
-  <si>
     <t>LED2</t>
   </si>
   <si>
@@ -324,16 +300,55 @@
   </si>
   <si>
     <t>14J7919</t>
+  </si>
+  <si>
+    <t>OC_DIGIKEY</t>
+  </si>
+  <si>
+    <t>768-1007-1-ND</t>
+  </si>
+  <si>
+    <t>ATMEGA168-20AU-ND</t>
+  </si>
+  <si>
+    <t>FTDI USB chip</t>
+  </si>
+  <si>
+    <t>490-1198-1-ND</t>
+  </si>
+  <si>
+    <t>QTY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -356,13 +371,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -645,26 +664,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -690,565 +708,542 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="E8" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="J8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>24</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>25</v>
       </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="E8" t="s">
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="I10" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-      <c r="E9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E11" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="I11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E13" t="s">
         <v>35</v>
       </c>
-      <c r="G11" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="s">
         <v>33</v>
       </c>
-      <c r="H11">
-        <v>1146032</v>
-      </c>
-      <c r="I11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="D14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>38</v>
       </c>
-      <c r="D12" t="s">
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="E12" t="s">
+      <c r="D15" t="s">
         <v>40</v>
       </c>
-      <c r="J12" t="s">
+      <c r="E15" t="s">
         <v>41</v>
       </c>
-      <c r="K12" t="s">
+      <c r="H15" t="s">
         <v>42</v>
       </c>
-      <c r="L12" t="s">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B16" t="s">
         <v>44</v>
       </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" t="s">
-        <v>40</v>
-      </c>
-      <c r="J13" t="s">
-        <v>41</v>
-      </c>
-      <c r="K13" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="C16" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" t="s">
-        <v>41</v>
-      </c>
-      <c r="K14" t="s">
-        <v>42</v>
-      </c>
-      <c r="L14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="D16" t="s">
         <v>46</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E16" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>48</v>
       </c>
-      <c r="E15" t="s">
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>49</v>
       </c>
-      <c r="H15" t="s">
+      <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="I15" t="s">
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>52</v>
-      </c>
-      <c r="C16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D16" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>60</v>
       </c>
       <c r="B20">
         <v>680</v>
       </c>
       <c r="C20" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>63</v>
       </c>
       <c r="B21">
         <v>680</v>
       </c>
       <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>58</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+      <c r="E25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
         <v>61</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D26" t="s">
         <v>62</v>
       </c>
-      <c r="E21" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="E26" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" t="s">
         <v>64</v>
       </c>
-      <c r="B22" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="H26" t="s">
         <v>65</v>
       </c>
-      <c r="B23" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>66</v>
       </c>
-      <c r="B24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B27" t="s">
         <v>67</v>
       </c>
-      <c r="B25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C27" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>68</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B28" t="s">
         <v>69</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" t="s">
         <v>70</v>
       </c>
-      <c r="E26" t="s">
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>71</v>
       </c>
-      <c r="G26" t="s">
+      <c r="B29" t="s">
         <v>72</v>
       </c>
-      <c r="H26">
-        <v>176432</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B30" t="s">
         <v>74</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" t="s">
         <v>75</v>
       </c>
-      <c r="C27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="E30" t="s">
         <v>76</v>
       </c>
-      <c r="B28" t="s">
+      <c r="H30" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>77</v>
       </c>
-      <c r="C28" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="B31" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="C31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" t="s">
         <v>79</v>
       </c>
-      <c r="B29" t="s">
+      <c r="F31" t="s">
         <v>80</v>
       </c>
-      <c r="C29" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="G31" t="s">
         <v>81</v>
       </c>
-      <c r="B30" t="s">
+      <c r="H31" t="s">
         <v>82</v>
-      </c>
-      <c r="C30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" t="s">
-        <v>84</v>
-      </c>
-      <c r="H30" t="s">
-        <v>50</v>
-      </c>
-      <c r="I30" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>85</v>
-      </c>
-      <c r="B31" t="s">
-        <v>86</v>
-      </c>
-      <c r="C31" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" t="s">
-        <v>87</v>
-      </c>
-      <c r="F31" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" t="s">
-        <v>89</v>
-      </c>
-      <c r="H31">
-        <v>4195115</v>
-      </c>
-      <c r="I31" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>